<commit_message>
starting to fix bugs in this app
</commit_message>
<xml_diff>
--- a/app/data/Course_Data.xlsx
+++ b/app/data/Course_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://meridianenergy-my.sharepoint.com/personal/russell_chubb_meridianenergy_co_nz/Documents/Documents/Programming/Personal/Golf_Stats_App/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://meridianenergy-my.sharepoint.com/personal/russell_chubb_meridianenergy_co_nz/Documents/Documents/Programming/Personal/Golf_Stats_App/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_F25DC773A252ABDACC104822F95A42B45BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A929883-5787-4CD0-B7F1-8D5D8CC3506D}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_F25DC773A252ABDACC104822F95A42B45BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A6B3D8F-F872-4B11-A73F-98C25E723432}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="870" windowWidth="14400" windowHeight="8180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Course" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="7">
   <si>
     <t>Course</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Golf Warehouse</t>
+  </si>
+  <si>
+    <t>Masterton Golf Course</t>
   </si>
 </sst>
 </file>
@@ -105,10 +108,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -374,13 +373,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -774,6 +776,258 @@
         <v>113</v>
       </c>
     </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>6</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41">
+        <v>13</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <v>14</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <v>15</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44">
+        <v>16</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45">
+        <v>17</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>18</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>453</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>